<commit_message>
add title to description section
</commit_message>
<xml_diff>
--- a/dist/assets/data/glioma.xlsx
+++ b/dist/assets/data/glioma.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/devlan/Repos/research/data-forensics/dist/assets/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BAFBDFED-C1F0-224D-BCB8-0CA14043BEC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F390E0-FA3A-0F42-BCDB-7E918DFA6253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2180" yWindow="4380" windowWidth="26920" windowHeight="12520"/>
+    <workbookView xWindow="5600" yWindow="3860" windowWidth="26920" windowHeight="12520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,21 +18,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="114210"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="276">
   <si>
     <t>NM_007423</t>
   </si>
@@ -850,9 +840,6 @@
     <t>Functional Gene Grouping (II)</t>
   </si>
   <si>
-    <t>Supplementary Table 2. Mouse embryonic stem cell array PAMM-081A: Mouse iPS cells relative to mouse embryonic fibroblasts</t>
-  </si>
-  <si>
     <t>Parietal endoderm marker</t>
   </si>
   <si>
@@ -863,19 +850,16 @@
   </si>
   <si>
     <t>ESC differentiation/lineage markers</t>
-  </si>
-  <si>
-    <t>This Supporting Information file has been retracted (08/21/2019)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -897,12 +881,6 @@
     <font>
       <b/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -962,7 +940,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
@@ -970,13 +948,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -1021,9 +999,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1303,11 +1278,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G87"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1322,48 +1297,78 @@
     <col min="8" max="256" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A1" s="24" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="25" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="14" x14ac:dyDescent="0.15">
-      <c r="A3" s="15" t="s">
+    <row r="1" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+      <c r="A1" s="15" t="s">
         <v>266</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B1" s="16" t="s">
         <v>267</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C1" s="17" t="s">
         <v>268</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D1" s="18" t="s">
         <v>269</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E1" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F1" s="14" t="s">
         <v>271</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="12">
+        <v>14.793799999999999</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="12">
+        <v>0.46360000000000001</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="D4" s="12">
-        <v>14.793799999999999</v>
+        <v>50.509</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>253</v>
@@ -1374,16 +1379,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>72</v>
+        <v>150</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>73</v>
+        <v>151</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>74</v>
+        <v>152</v>
       </c>
       <c r="D5" s="12">
-        <v>0.46360000000000001</v>
+        <v>272.79070000000002</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>253</v>
@@ -1394,36 +1399,36 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>75</v>
+        <v>164</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>76</v>
+        <v>165</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>77</v>
+        <v>166</v>
       </c>
       <c r="D6" s="12">
-        <v>50.509</v>
+        <v>150.52080000000001</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>150</v>
+        <v>167</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>151</v>
+        <v>168</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>152</v>
+        <v>169</v>
       </c>
       <c r="D7" s="12">
-        <v>272.79070000000002</v>
+        <v>14.467000000000001</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>253</v>
@@ -1434,176 +1439,176 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>164</v>
+        <v>191</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="D8" s="12">
-        <v>150.52080000000001</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="F8" t="s">
+        <v>2017.5435</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>167</v>
+        <v>218</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>168</v>
+        <v>219</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>169</v>
+        <v>220</v>
       </c>
       <c r="D9" s="12">
-        <v>14.467000000000001</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="F9" s="9" t="s">
+        <v>218.40539999999999</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>191</v>
+        <v>233</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>192</v>
+        <v>234</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>193</v>
+        <v>235</v>
       </c>
       <c r="D10" s="12">
-        <v>2017.5435</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="F10" s="11" t="s">
+        <v>228.8357</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>218</v>
+        <v>242</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>219</v>
+        <v>243</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>220</v>
+        <v>244</v>
       </c>
       <c r="D11" s="12">
-        <v>218.40539999999999</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="F11" s="11" t="s">
+        <v>1194.5975000000001</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="F11" s="10" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>233</v>
+        <v>248</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>235</v>
+        <v>250</v>
       </c>
       <c r="D12" s="12">
-        <v>228.8357</v>
+        <v>1106.6193000000001</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="9" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>242</v>
+        <v>21</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>243</v>
+        <v>22</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>244</v>
+        <v>23</v>
       </c>
       <c r="D13" s="12">
-        <v>1194.5975000000001</v>
+        <v>0.31919999999999998</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="F13" s="10" t="s">
-        <v>251</v>
+      <c r="F13" s="6" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>248</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>249</v>
+        <v>25</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>250</v>
+        <v>26</v>
       </c>
       <c r="D14" s="12">
-        <v>1106.6193000000001</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>251</v>
+        <v>0.33810000000000001</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="D15" s="12">
-        <v>0.31919999999999998</v>
+        <v>0.17979999999999999</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="8" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="D16" s="12">
-        <v>0.33810000000000001</v>
+        <v>346.58159999999998</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>253</v>
@@ -1614,76 +1619,76 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D17" s="12">
-        <v>0.17979999999999999</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="F17" s="8" t="s">
+        <v>0.7147</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="D18" s="12">
-        <v>346.58159999999998</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="F18" s="2" t="s">
+        <v>2.8776999999999999</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="F18" s="6" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="D19" s="12">
-        <v>0.7147</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="F19" s="2" t="s">
+        <v>5.0343</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="F19" s="7" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="D20" s="12">
-        <v>2.8776999999999999</v>
+        <v>27.4283</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>253</v>
@@ -1694,118 +1699,118 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>66</v>
+        <v>96</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>67</v>
+        <v>97</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="D21" s="12">
-        <v>5.0343</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="F21" s="7" t="s">
+        <v>2.9868999999999999</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="F21" s="8" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="D22" s="12">
-        <v>27.4283</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="F22" s="6" t="s">
+        <v>27.154599999999999</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="D23" s="12">
-        <v>2.9868999999999999</v>
+        <v>0.9224</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="F23" s="2" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="D24" s="12">
-        <v>27.154599999999999</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="F24" s="2" t="s">
+        <v>36.372100000000003</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="F24" s="8" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="D25" s="12">
-        <v>0.9224</v>
+        <v>212.84389999999999</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="8" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="D26" s="12">
-        <v>36.372100000000003</v>
-      </c>
-      <c r="E26" s="4" t="s">
+        <v>287.4606</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>253</v>
       </c>
       <c r="F26" s="8" t="s">
@@ -1814,38 +1819,38 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="D27" s="12">
-        <v>212.84389999999999</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="F27" s="8" t="s">
+        <v>0.15620000000000001</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="F27" s="6" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
-        <v>135</v>
+        <v>159</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>136</v>
+        <v>160</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>137</v>
+        <v>160</v>
       </c>
       <c r="D28" s="12">
-        <v>287.4606</v>
-      </c>
-      <c r="E28" s="3" t="s">
+        <v>40.648600000000002</v>
+      </c>
+      <c r="E28" s="4" t="s">
         <v>253</v>
       </c>
       <c r="F28" s="8" t="s">
@@ -1854,18 +1859,18 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
-        <v>138</v>
+        <v>161</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>139</v>
+        <v>162</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="D29" s="12">
-        <v>0.15620000000000001</v>
-      </c>
-      <c r="E29" s="4" t="s">
+        <v>0.1023</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>253</v>
       </c>
       <c r="F29" s="6" t="s">
@@ -1874,38 +1879,38 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="D30" s="12">
-        <v>40.648600000000002</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="F30" s="8" t="s">
+        <v>0.53520000000000001</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
-        <v>161</v>
+        <v>194</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>162</v>
+        <v>195</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>163</v>
+        <v>196</v>
       </c>
       <c r="D31" s="12">
-        <v>0.1023</v>
-      </c>
-      <c r="E31" s="3" t="s">
+        <v>0.41610000000000003</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>253</v>
       </c>
       <c r="F31" s="6" t="s">
@@ -1914,176 +1919,176 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
-        <v>170</v>
+        <v>212</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>171</v>
+        <v>213</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>172</v>
+        <v>214</v>
       </c>
       <c r="D32" s="12">
-        <v>0.53520000000000001</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="F32" s="2" t="s">
+        <v>0.1661</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="F32" s="8" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
-        <v>194</v>
+        <v>236</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>195</v>
+        <v>237</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>196</v>
+        <v>238</v>
       </c>
       <c r="D33" s="12">
-        <v>0.41610000000000003</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="F33" s="6" t="s">
+        <v>897.21669999999995</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
-        <v>212</v>
+        <v>3</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>213</v>
+        <v>4</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>214</v>
+        <v>5</v>
       </c>
       <c r="D34" s="12">
-        <v>0.1661</v>
+        <v>1.2078</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="F34" s="8" t="s">
-        <v>252</v>
+      <c r="F34" s="2" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
-        <v>236</v>
+        <v>9</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>237</v>
+        <v>10</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>238</v>
+        <v>11</v>
       </c>
       <c r="D35" s="12">
-        <v>897.21669999999995</v>
+        <v>0.59889999999999999</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>253</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="D36" s="12">
-        <v>1.2078</v>
+        <v>1.1919</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F36" s="6" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D37" s="12">
-        <v>0.59889999999999999</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="F37" s="2" t="s">
+        <v>15.6366</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="F37" s="6" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
-        <v>33</v>
+        <v>105</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>34</v>
+        <v>106</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>35</v>
+        <v>107</v>
       </c>
       <c r="D38" s="12">
-        <v>1.1919</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="F38" s="6" t="s">
+        <v>0.83630000000000004</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
-        <v>36</v>
+        <v>108</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>37</v>
+        <v>109</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>38</v>
+        <v>110</v>
       </c>
       <c r="D39" s="12">
-        <v>15.6366</v>
+        <v>0.86950000000000005</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="F39" s="6" t="s">
+      <c r="F39" s="2" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
-        <v>105</v>
+        <v>141</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>106</v>
+        <v>142</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="D40" s="12">
-        <v>0.83630000000000004</v>
+        <v>100.8125</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>253</v>
@@ -2094,76 +2099,76 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
-        <v>108</v>
+        <v>188</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>109</v>
+        <v>189</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>110</v>
+        <v>190</v>
       </c>
       <c r="D41" s="12">
-        <v>0.86950000000000005</v>
+        <v>35.134599999999999</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="F41" s="8" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
-        <v>141</v>
+        <v>200</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>142</v>
+        <v>201</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>143</v>
+        <v>202</v>
       </c>
       <c r="D42" s="12">
-        <v>100.8125</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="F42" s="2" t="s">
+        <v>1.5946</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="F42" s="7" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
-        <v>188</v>
+        <v>206</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>189</v>
+        <v>207</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="D43" s="12">
-        <v>35.134599999999999</v>
+        <v>1.4800000000000001E-2</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="F43" s="8" t="s">
+      <c r="F43" s="7" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
-        <v>200</v>
+        <v>239</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>201</v>
+        <v>240</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>202</v>
+        <v>241</v>
       </c>
       <c r="D44" s="12">
-        <v>1.5946</v>
+        <v>1.8775999999999999</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>253</v>
@@ -2174,18 +2179,18 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
-        <v>206</v>
+        <v>84</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>207</v>
+        <v>85</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>208</v>
+        <v>86</v>
       </c>
       <c r="D45" s="12">
-        <v>1.4800000000000001E-2</v>
-      </c>
-      <c r="E45" s="4" t="s">
+        <v>48.2211</v>
+      </c>
+      <c r="E45" s="3" t="s">
         <v>253</v>
       </c>
       <c r="F45" s="7" t="s">
@@ -2194,849 +2199,806 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
-        <v>239</v>
+        <v>0</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>240</v>
+        <v>1</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>241</v>
+        <v>2</v>
       </c>
       <c r="D46" s="12">
-        <v>1.8775999999999999</v>
+        <v>5.2916999999999996</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>254</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="F46" s="19" t="s">
+        <v>274</v>
+      </c>
+      <c r="G46" s="2"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
-        <v>84</v>
+        <v>209</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>85</v>
+        <v>210</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>86</v>
+        <v>211</v>
       </c>
       <c r="D47" s="12">
-        <v>48.2211</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>254</v>
+        <v>4.8205999999999998</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="F47" s="19" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D48" s="12">
-        <v>5.2916999999999996</v>
+        <v>6.6428000000000003</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F48" s="19" t="s">
-        <v>275</v>
-      </c>
-      <c r="G48" s="2"/>
+        <v>256</v>
+      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
-        <v>209</v>
+        <v>42</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>210</v>
+        <v>43</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>211</v>
+        <v>44</v>
       </c>
       <c r="D49" s="12">
-        <v>4.8205999999999998</v>
+        <v>26.037700000000001</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F49" s="19" t="s">
-        <v>275</v>
+        <v>275</v>
+      </c>
+      <c r="F49" s="20" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>16</v>
+        <v>82</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="D50" s="12">
-        <v>6.6428000000000003</v>
+        <v>8.6956000000000007</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F50" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="F50" s="21" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
-        <v>42</v>
+        <v>120</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>43</v>
+        <v>121</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>44</v>
+        <v>122</v>
       </c>
       <c r="D51" s="12">
-        <v>26.037700000000001</v>
+        <v>8.0067000000000004</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F51" s="20" t="s">
+        <v>275</v>
+      </c>
+      <c r="F51" s="21" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="D52" s="12">
-        <v>8.6956000000000007</v>
+        <v>3.2099999999999997E-2</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F52" s="21" t="s">
-        <v>256</v>
+        <v>275</v>
+      </c>
+      <c r="F52" s="22" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D53" s="12">
-        <v>8.0067000000000004</v>
+        <v>21.2864</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F53" s="21" t="s">
-        <v>256</v>
+        <v>275</v>
+      </c>
+      <c r="F53" s="22" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
-        <v>54</v>
+        <v>126</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>55</v>
+        <v>127</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>56</v>
+        <v>128</v>
       </c>
       <c r="D54" s="12">
-        <v>3.2099999999999997E-2</v>
+        <v>0.26440000000000002</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F54" s="22" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="D55" s="12">
-        <v>21.2864</v>
+        <v>7.8700000000000006E-2</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F55" s="22" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
-        <v>126</v>
+        <v>215</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>127</v>
+        <v>216</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>128</v>
+        <v>217</v>
       </c>
       <c r="D56" s="12">
-        <v>0.26440000000000002</v>
+        <v>4.8205999999999998</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F56" s="22" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="s">
-        <v>129</v>
+        <v>78</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>131</v>
+        <v>80</v>
       </c>
       <c r="D57" s="12">
-        <v>7.8700000000000006E-2</v>
+        <v>4.8205999999999998</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F57" s="22" t="s">
+        <v>275</v>
+      </c>
+      <c r="F57" s="23" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
-        <v>215</v>
+        <v>99</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>216</v>
+        <v>100</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>217</v>
+        <v>101</v>
       </c>
       <c r="D58" s="12">
         <v>4.8205999999999998</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F58" s="22" t="s">
+        <v>275</v>
+      </c>
+      <c r="F58" s="23" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>79</v>
+        <v>115</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>80</v>
+        <v>116</v>
       </c>
       <c r="D59" s="12">
         <v>4.8205999999999998</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F59" s="23" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
-        <v>99</v>
+        <v>176</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>100</v>
+        <v>177</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>101</v>
+        <v>178</v>
       </c>
       <c r="D60" s="12">
         <v>4.8205999999999998</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F60" s="23" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
-        <v>114</v>
+        <v>182</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>115</v>
+        <v>183</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>116</v>
+        <v>184</v>
       </c>
       <c r="D61" s="12">
-        <v>4.8205999999999998</v>
+        <v>5.0450999999999997</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F61" s="23" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
-        <v>176</v>
+        <v>221</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>177</v>
+        <v>222</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>178</v>
+        <v>223</v>
       </c>
       <c r="D62" s="12">
         <v>4.8205999999999998</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F62" s="23" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="D63" s="12">
-        <v>5.0450999999999997</v>
+        <v>4.8205999999999998</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F63" s="23" t="s">
-        <v>274</v>
+        <v>275</v>
+      </c>
+      <c r="F63" s="11" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A64" s="1" t="s">
-        <v>221</v>
+        <v>230</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="D64" s="12">
         <v>4.8205999999999998</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F64" s="23" t="s">
-        <v>274</v>
+        <v>275</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A65" s="1" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="D65" s="12">
-        <v>4.8205999999999998</v>
+        <v>7.5399999999999995E-2</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F65" s="11" t="s">
-        <v>265</v>
+        <v>275</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A66" s="1" t="s">
-        <v>230</v>
+        <v>156</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>231</v>
+        <v>157</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>232</v>
+        <v>158</v>
       </c>
       <c r="D66" s="12">
-        <v>4.8205999999999998</v>
+        <v>26.728999999999999</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F66" s="6" t="s">
-        <v>265</v>
+        <v>275</v>
+      </c>
+      <c r="F66" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
-        <v>153</v>
+        <v>179</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>154</v>
+        <v>180</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>155</v>
+        <v>181</v>
       </c>
       <c r="D67" s="12">
-        <v>7.5399999999999995E-2</v>
+        <v>6.2587999999999999</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F67" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="F67" s="11" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
-        <v>156</v>
+        <v>30</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>157</v>
+        <v>31</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>158</v>
+        <v>32</v>
       </c>
       <c r="D68" s="12">
-        <v>26.728999999999999</v>
+        <v>0.1522</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F68" t="s">
-        <v>262</v>
+        <v>275</v>
+      </c>
+      <c r="F68" s="8" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
-        <v>179</v>
+        <v>144</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>180</v>
+        <v>145</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>181</v>
+        <v>146</v>
       </c>
       <c r="D69" s="12">
-        <v>6.2587999999999999</v>
+        <v>4.8205999999999998</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F69" s="11" t="s">
-        <v>262</v>
+        <v>275</v>
+      </c>
+      <c r="F69" s="9" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>31</v>
+        <v>148</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>32</v>
+        <v>149</v>
       </c>
       <c r="D70" s="12">
-        <v>0.1522</v>
+        <v>0.89890000000000003</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F70" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="F70" s="9" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
-        <v>144</v>
+        <v>227</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>145</v>
+        <v>228</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>146</v>
+        <v>229</v>
       </c>
       <c r="D71" s="12">
-        <v>4.8205999999999998</v>
+        <v>97.186199999999999</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F71" s="9" t="s">
-        <v>259</v>
+        <v>275</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A72" s="1" t="s">
-        <v>147</v>
+        <v>245</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>148</v>
+        <v>246</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>149</v>
+        <v>247</v>
       </c>
       <c r="D72" s="12">
-        <v>0.89890000000000003</v>
+        <v>1.2919</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F72" s="9" t="s">
-        <v>259</v>
+        <v>275</v>
+      </c>
+      <c r="F72" s="11" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A73" s="1" t="s">
-        <v>227</v>
+        <v>27</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>228</v>
+        <v>28</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>229</v>
+        <v>29</v>
       </c>
       <c r="D73" s="12">
-        <v>97.186199999999999</v>
+        <v>7.4653999999999998</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F73" s="6" t="s">
-        <v>258</v>
+        <v>275</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A74" s="1" t="s">
-        <v>245</v>
+        <v>224</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>246</v>
+        <v>225</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
       <c r="D74" s="12">
-        <v>1.2919</v>
+        <v>140.2405</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F74" s="11" t="s">
-        <v>258</v>
+        <v>275</v>
+      </c>
+      <c r="F74" s="10" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A75" s="1" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="D75" s="12">
-        <v>7.4653999999999998</v>
+        <v>4.7736999999999998</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>264</v>
+        <v>275</v>
+      </c>
+      <c r="F75" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A76" s="1" t="s">
-        <v>224</v>
+        <v>197</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>225</v>
+        <v>198</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>226</v>
+        <v>199</v>
       </c>
       <c r="D76" s="12">
-        <v>140.2405</v>
+        <v>4.8205999999999998</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F76" s="10" t="s">
-        <v>264</v>
+        <v>275</v>
+      </c>
+      <c r="F76" s="11" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A77" s="1" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D77" s="12">
-        <v>4.7736999999999998</v>
+        <v>4.8205999999999998</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F77" t="s">
-        <v>255</v>
+        <v>275</v>
+      </c>
+      <c r="F77" s="8" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A78" s="1" t="s">
-        <v>197</v>
+        <v>6</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>198</v>
+        <v>7</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>199</v>
+        <v>8</v>
       </c>
       <c r="D78" s="12">
-        <v>4.8205999999999998</v>
+        <v>0.1356</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F78" s="11" t="s">
-        <v>255</v>
+        <v>275</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A79" s="1" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="D79" s="12">
-        <v>4.8205999999999998</v>
+        <v>2.0680000000000001</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F79" s="8" t="s">
-        <v>257</v>
+        <v>275</v>
+      </c>
+      <c r="F79" s="6" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A80" s="1" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="D80" s="12">
-        <v>0.1356</v>
+        <v>0.32300000000000001</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F80" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="F80" s="8" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A81" s="1" t="s">
-        <v>12</v>
+        <v>185</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>13</v>
+        <v>186</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>14</v>
+        <v>187</v>
       </c>
       <c r="D81" s="12">
-        <v>2.0680000000000001</v>
+        <v>79.054000000000002</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F81" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="F81" s="2" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A82" s="1" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="D82" s="12">
-        <v>0.32300000000000001</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F82" s="8" t="s">
-        <v>263</v>
+        <v>275</v>
+      </c>
+      <c r="F82" s="6" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A83" s="1" t="s">
-        <v>185</v>
+        <v>203</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>186</v>
+        <v>204</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>187</v>
+        <v>205</v>
       </c>
       <c r="D83" s="12">
-        <v>79.054000000000002</v>
+        <v>3.85E-2</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F83" s="2" t="s">
-        <v>263</v>
+        <v>275</v>
+      </c>
+      <c r="F83" s="8" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A84" s="1" t="s">
-        <v>18</v>
+        <v>90</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>19</v>
+        <v>91</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="D84" s="12">
-        <v>5.0000000000000001E-4</v>
+        <v>4.8205999999999998</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F84" s="6" t="s">
-        <v>261</v>
+        <v>275</v>
+      </c>
+      <c r="F84" s="8" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A85" s="1" t="s">
-        <v>203</v>
+        <v>93</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>204</v>
+        <v>94</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>205</v>
+        <v>95</v>
       </c>
       <c r="D85" s="12">
-        <v>3.85E-2</v>
+        <v>4.9755000000000003</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F85" s="8" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A86" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D86" s="12">
-        <v>4.8205999999999998</v>
-      </c>
-      <c r="E86" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F86" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="F85" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A87" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D87" s="12">
-        <v>4.9755000000000003</v>
-      </c>
-      <c r="E87" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F87" t="s">
-        <v>260</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:XFD2"/>
-  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -3045,7 +3007,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3062,7 +3024,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
remove empty rows/columns convert csv to xlsx
</commit_message>
<xml_diff>
--- a/dist/assets/data/glioma.xlsx
+++ b/dist/assets/data/glioma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/devlan/Repos/research/data-forensics/dist/assets/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F390E0-FA3A-0F42-BCDB-7E918DFA6253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6331CD05-484C-3542-B592-7251EF9EB87C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5600" yWindow="3860" windowWidth="26920" windowHeight="12520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1279,10 +1279,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G85"/>
+  <dimension ref="A1:F85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1290,11 +1290,10 @@
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="8.83203125" customWidth="1"/>
     <col min="3" max="3" width="73.1640625" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="50.33203125" style="13" customWidth="1"/>
     <col min="5" max="5" width="31.1640625" style="5" customWidth="1"/>
     <col min="6" max="6" width="53.33203125" customWidth="1"/>
-    <col min="7" max="7" width="26.33203125" customWidth="1"/>
-    <col min="8" max="256" width="8.83203125" customWidth="1"/>
+    <col min="7" max="255" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -1937,7 +1936,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>236</v>
       </c>
@@ -1957,7 +1956,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>3</v>
       </c>
@@ -1977,7 +1976,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>9</v>
       </c>
@@ -1997,7 +1996,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>33</v>
       </c>
@@ -2017,7 +2016,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -2037,7 +2036,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>105</v>
       </c>
@@ -2057,7 +2056,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>108</v>
       </c>
@@ -2077,7 +2076,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>141</v>
       </c>
@@ -2097,7 +2096,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>188</v>
       </c>
@@ -2117,7 +2116,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
         <v>200</v>
       </c>
@@ -2137,7 +2136,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>206</v>
       </c>
@@ -2157,7 +2156,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>239</v>
       </c>
@@ -2177,7 +2176,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
         <v>84</v>
       </c>
@@ -2197,7 +2196,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
         <v>0</v>
       </c>
@@ -2216,9 +2215,8 @@
       <c r="F46" s="19" t="s">
         <v>274</v>
       </c>
-      <c r="G46" s="2"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
         <v>209</v>
       </c>
@@ -2238,7 +2236,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Paper push 1 (#130)
* add logic to be able to switch between including and not include data format in styling.

* minor ui tweaks

* remove empty rows/columns convert csv to xlsx

* update title/icon and intro sentence

* update to minimum landing page

* convert csv to xlsx

* update chart images

* update figures and short descriptions

* fix broken link

* remove broken upload button minor tweaks

* remove lipsum
</commit_message>
<xml_diff>
--- a/dist/assets/data/glioma.xlsx
+++ b/dist/assets/data/glioma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/devlan/Repos/research/data-forensics/dist/assets/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F390E0-FA3A-0F42-BCDB-7E918DFA6253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6331CD05-484C-3542-B592-7251EF9EB87C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5600" yWindow="3860" windowWidth="26920" windowHeight="12520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1279,10 +1279,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G85"/>
+  <dimension ref="A1:F85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1290,11 +1290,10 @@
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="8.83203125" customWidth="1"/>
     <col min="3" max="3" width="73.1640625" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="50.33203125" style="13" customWidth="1"/>
     <col min="5" max="5" width="31.1640625" style="5" customWidth="1"/>
     <col min="6" max="6" width="53.33203125" customWidth="1"/>
-    <col min="7" max="7" width="26.33203125" customWidth="1"/>
-    <col min="8" max="256" width="8.83203125" customWidth="1"/>
+    <col min="7" max="255" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -1937,7 +1936,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>236</v>
       </c>
@@ -1957,7 +1956,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>3</v>
       </c>
@@ -1977,7 +1976,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>9</v>
       </c>
@@ -1997,7 +1996,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>33</v>
       </c>
@@ -2017,7 +2016,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -2037,7 +2036,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>105</v>
       </c>
@@ -2057,7 +2056,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>108</v>
       </c>
@@ -2077,7 +2076,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>141</v>
       </c>
@@ -2097,7 +2096,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>188</v>
       </c>
@@ -2117,7 +2116,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
         <v>200</v>
       </c>
@@ -2137,7 +2136,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>206</v>
       </c>
@@ -2157,7 +2156,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>239</v>
       </c>
@@ -2177,7 +2176,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
         <v>84</v>
       </c>
@@ -2197,7 +2196,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
         <v>0</v>
       </c>
@@ -2216,9 +2215,8 @@
       <c r="F46" s="19" t="s">
         <v>274</v>
       </c>
-      <c r="G46" s="2"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
         <v>209</v>
       </c>
@@ -2238,7 +2236,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
         <v>15</v>
       </c>

</xml_diff>